<commit_message>
Auto update nse_indices_1 outputs
</commit_message>
<xml_diff>
--- a/nse_indices_1_dashboard.xlsx
+++ b/nse_indices_1_dashboard.xlsx
@@ -502,7 +502,7 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>5.5%</t>
+          <t>5.55%</t>
         </is>
       </c>
     </row>
@@ -614,21 +614,21 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>Nifty 50</t>
+          <t>Nifty Midcap 100</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>6.34</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>Nifty Midcap 100</t>
+          <t>Nifty 50</t>
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>6.11</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="5">
@@ -810,7 +810,7 @@
         <v>17383</v>
       </c>
       <c r="G2" s="8" t="n">
-        <v>60299.80078125</v>
+        <v>60594.6015625</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>22207.900390625</v>
@@ -3244,7 +3244,7 @@
         <v>8.42</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>6.11</v>
+        <v>6.63</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>5.19</v>
@@ -5690,7 +5690,7 @@
         <v>0.76</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>0.39</v>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>Nifty Midcap 100, Nifty500 Multicap 50:25:25, Nifty Next 50</t>
+          <t>Nifty500 Multicap 50:25:25, Nifty Next 50, Nifty Midcap 150</t>
         </is>
       </c>
     </row>

</xml_diff>